<commit_message>
Adding Date of  Birth to participant signups, part 3
</commit_message>
<xml_diff>
--- a/test/fixtures/files/invalid_participant.xlsx
+++ b/test/fixtures/files/invalid_participant.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="54">
   <si>
     <t xml:space="preserve">RowID</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t xml:space="preserve">Status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOB</t>
   </si>
   <si>
     <t xml:space="preserve">Age</t>
@@ -194,6 +197,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -279,16 +283,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AP2"/>
+  <dimension ref="A1:AQ2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.46"/>
@@ -297,37 +301,37 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="6.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="4.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="7.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="5.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="11.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="9.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="9.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="12.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="6.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="19.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="8.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="14.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="11.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="13.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="9.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="6.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="6.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="28" style="0" width="5.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="6.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="6.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="8.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="12.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="13.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="9.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="7.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="8.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="8.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="0" width="11.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="0" width="10.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="0" width="4.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="7.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="5.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="11.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="9.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="9.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="12.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="6.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="19.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="8.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="14.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="10.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="11.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="13.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="9.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="6.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="6.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="29" style="0" width="5.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="6.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="6.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="11.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="8.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="12.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="13.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="9.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="11.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="7.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="8.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="0" width="8.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="0" width="11.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="0" width="10.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -457,82 +461,86 @@
       <c r="AP1" s="0" t="s">
         <v>41</v>
       </c>
+      <c r="AQ1" s="0" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>-437868471</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G2" s="0" t="n">
         <v>35</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>45</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="K2" s="1"/>
       <c r="L2" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="N2" s="0" t="s">
-        <v>49</v>
+        <v>46</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="O2" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="P2" s="0" t="n">
+      <c r="P2" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q2" s="0" t="n">
         <v>3195</v>
       </c>
-      <c r="Q2" s="0" t="n">
+      <c r="R2" s="0" t="n">
         <v>61434006439</v>
       </c>
-      <c r="S2" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y2" s="1" t="s">
+      <c r="T2" s="0" t="s">
         <v>52</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AB2" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="AD2" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="AE2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AG2" s="1" t="s">
-        <v>45</v>
+        <v>53</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Injuries field to admin participant download  and import
</commit_message>
<xml_diff>
--- a/test/fixtures/files/invalid_participant.xlsx
+++ b/test/fixtures/files/invalid_participant.xlsx
@@ -160,7 +160,7 @@
     <t>EmergEmail</t>
   </si>
   <si>
-    <t>CampPrefs</t>
+    <t>Injuiries</t>
   </si>
   <si>
     <t>CAF</t>
@@ -210,13 +210,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -252,7 +258,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -263,13 +269,22 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -583,59 +598,59 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="6" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="6.433571428571429" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="9.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="7" width="5.433571428571429" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="7" width="9.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="6" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="7" width="7.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="7" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="7" width="6.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="7" width="4.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="7" width="4.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="7" width="7.433571428571429" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="7" width="5.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="7" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="7" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="8" width="6.433571428571429" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="8" width="9.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="8" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="8" width="5.433571428571429" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="8" width="9.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="7" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="8" width="7.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="8" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="8" width="6.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="9" width="4.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="8" width="4.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="8" width="7.433571428571429" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="8" width="5.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="10" width="11.862142857142858" customWidth="1" bestFit="1"/>
     <col min="16" max="16" style="7" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="7" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="7" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="7" width="11.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="7" width="9.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="6" width="9.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="22" max="22" style="6" width="12.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="23" max="23" style="7" width="6.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="24" max="24" style="7" width="19.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="25" max="25" style="7" width="9.005" customWidth="1" bestFit="1"/>
-    <col min="26" max="26" style="7" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="27" max="27" style="7" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="28" max="28" style="7" width="11.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="29" max="29" style="7" width="13.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="30" max="30" style="7" width="9.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="31" max="31" style="7" width="6.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="32" max="32" style="7" width="6.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="33" max="33" style="7" width="5.433571428571429" customWidth="1" bestFit="1"/>
-    <col min="34" max="34" style="7" width="5.433571428571429" customWidth="1" bestFit="1"/>
-    <col min="35" max="35" style="7" width="6.433571428571429" customWidth="1" bestFit="1"/>
-    <col min="36" max="36" style="7" width="6.2907142857142855" customWidth="1" bestFit="1"/>
-    <col min="37" max="37" style="7" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="38" max="38" style="7" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="39" max="39" style="7" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="40" max="40" style="7" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="41" max="41" style="7" width="9.005" customWidth="1" bestFit="1"/>
-    <col min="42" max="42" style="7" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="43" max="43" style="7" width="13.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="44" max="44" style="7" width="9.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="45" max="45" style="7" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="46" max="46" style="7" width="7.433571428571429" customWidth="1" bestFit="1"/>
-    <col min="47" max="47" style="7" width="8.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="48" max="48" style="7" width="8.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="49" max="49" style="7" width="11.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="50" max="50" style="7" width="10.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="10" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="10" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="8" width="11.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="8" width="9.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="7" width="9.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="7" width="12.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" style="10" width="6.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="24" max="24" style="8" width="19.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="25" max="25" style="10" width="9.005" customWidth="1" bestFit="1"/>
+    <col min="26" max="26" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="27" max="27" style="10" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="28" max="28" style="10" width="11.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="29" max="29" style="10" width="13.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="30" max="30" style="8" width="9.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="31" max="31" style="8" width="6.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="32" max="32" style="10" width="6.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="33" max="33" style="8" width="5.433571428571429" customWidth="1" bestFit="1"/>
+    <col min="34" max="34" style="8" width="5.433571428571429" customWidth="1" bestFit="1"/>
+    <col min="35" max="35" style="8" width="6.433571428571429" customWidth="1" bestFit="1"/>
+    <col min="36" max="36" style="8" width="6.2907142857142855" customWidth="1" bestFit="1"/>
+    <col min="37" max="37" style="10" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="38" max="38" style="10" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="39" max="39" style="10" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="40" max="40" style="10" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="41" max="41" style="8" width="9.005" customWidth="1" bestFit="1"/>
+    <col min="42" max="42" style="10" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="43" max="43" style="10" width="13.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="44" max="44" style="10" width="9.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="45" max="45" style="10" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="46" max="46" style="10" width="7.433571428571429" customWidth="1" bestFit="1"/>
+    <col min="47" max="47" style="10" width="8.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="48" max="48" style="10" width="8.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="49" max="49" style="10" width="11.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="50" max="50" style="10" width="10.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -681,7 +696,7 @@
       <c r="O1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="4" t="s">
         <v>14</v>
       </c>
       <c r="Q1" s="3" t="s">
@@ -787,8 +802,8 @@
         <v>48</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="16.5">
-      <c r="A2" s="4">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="A2" s="5">
         <v>-437868471</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -806,7 +821,7 @@
       <c r="F2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="5">
         <v>35</v>
       </c>
       <c r="H2" s="2" t="s">
@@ -818,7 +833,7 @@
       <c r="J2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="K2" s="4"/>
+      <c r="K2" s="5"/>
       <c r="L2" s="2" t="s">
         <v>52</v>
       </c>
@@ -831,7 +846,7 @@
       <c r="O2" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="P2" s="5">
+      <c r="P2" s="6">
         <v>987654</v>
       </c>
       <c r="Q2" s="3" t="s">
@@ -846,10 +861,10 @@
       <c r="T2" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="U2" s="4">
+      <c r="U2" s="5">
         <v>3195</v>
       </c>
-      <c r="V2" s="4">
+      <c r="V2" s="5">
         <v>61434006439</v>
       </c>
       <c r="W2" s="3"/>

</xml_diff>